<commit_message>
Starting a Gradle Build Script
</commit_message>
<xml_diff>
--- a/me/1.Setting-up.xlsx
+++ b/me/1.Setting-up.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gradle\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48165A2E-DDCA-4362-AB95-0973227270CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F117327-1BEE-4C59-8923-8C20969894C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>https://www.oracle.com/java/technologies/downloads/#java8-windows</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>build.gradle</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>new project</t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,6 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7481,23 +7488,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D805BEE-7A8A-4610-959D-9618E4763899}">
   <dimension ref="A2:T960"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A733" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>40</v>
       </c>
@@ -7509,28 +7516,34 @@
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>42</v>
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="E8" t="s">
+      <c r="E8" s="16" t="s">
         <v>43</v>
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -7540,12 +7553,12 @@
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>36</v>
       </c>
@@ -7554,17 +7567,17 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>19</v>
       </c>

</xml_diff>